<commit_message>
Excel entry error caused error in plots
</commit_message>
<xml_diff>
--- a/Data/Fishers/FSP_Database_Fishers2223.xlsx
+++ b/Data/Fishers/FSP_Database_Fishers2223.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR13\Documents\LOCAL_NOT_ONEDRIVE\FSPsmallpelagics2022\Data\Fishers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D8FFC-215C-4AEF-BA1A-8E15418CEA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A3A25-DF1B-4297-89ED-FE1AFB613AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="21802" windowHeight="11756" tabRatio="727" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1333,9 +1333,9 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H27" sqref="H27"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A46:A67"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>30</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>30</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B26" t="s">
         <v>30</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B36" t="s">
         <v>30</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>30</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B39" t="s">
         <v>30</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B43" t="s">
         <v>30</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B45" t="s">
         <v>30</v>
@@ -3313,7 +3313,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B152"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
@@ -8801,7 +8801,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
@@ -12815,18 +12815,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12849,6 +12849,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20DD91-9730-4ADE-AA14-DA55753D06D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60DDBF2B-D2B5-4876-9C88-0C3D1310F83B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -12863,12 +12871,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E20DD91-9730-4ADE-AA14-DA55753D06D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>